<commit_message>
updates to data in DB
</commit_message>
<xml_diff>
--- a/excel/location.xlsx
+++ b/excel/location.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekty\for_work\ai-solution\ITSquad-antyfraud\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projekty\for_work\db-data\ITSquad-antyfraud\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{922B5847-2239-4BEA-905D-55CDE81FF712}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A2BCF1C-1B0D-475E-A3F9-818B635CB808}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="14400" yWindow="0" windowWidth="14400" windowHeight="15600" xr2:uid="{8302D55D-81BC-4BCF-A5C3-482C7184D220}"/>
   </bookViews>
@@ -3447,7 +3447,7 @@
   <dimension ref="A1:J384"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>